<commit_message>
make sure to have .csv files set to Copy always in copy to output directory to have release build work.
</commit_message>
<xml_diff>
--- a/RPGStoreSimulator/Inventory.xlsx
+++ b/RPGStoreSimulator/Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\treyp\source\repos\RPGStoreSimulator\RPGStoreSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF517CD3-1BDF-4479-AF48-3532603AAAD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E990F5-1CA5-42FA-80FA-749F18A74F0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14355" yWindow="3780" windowWidth="21600" windowHeight="11835" xr2:uid="{A509177C-1DC1-4F9D-B53C-458FC1853002}"/>
+    <workbookView xWindow="2490" yWindow="5940" windowWidth="21720" windowHeight="12435" xr2:uid="{A509177C-1DC1-4F9D-B53C-458FC1853002}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>weapontype</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>name</t>
   </si>
@@ -56,19 +53,16 @@
     <t>p</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>short sword</t>
-  </si>
-  <si>
-    <t>health potion</t>
-  </si>
-  <si>
     <t>bow</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>short_sword</t>
+  </si>
+  <si>
+    <t>health_potion</t>
   </si>
 </sst>
 </file>
@@ -423,7 +417,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,58 +429,61 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="C2">
         <v>10</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
         <v>10</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="C4">
         <v>12</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>